<commit_message>
Made typetest metadata only equal to typetest
</commit_message>
<xml_diff>
--- a/molgenis-app/src/test/resources/emx_all_datatypes_metadata_only.xlsx
+++ b/molgenis-app/src/test/resources/emx_all_datatypes_metadata_only.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="20480"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="83">
   <si>
     <t>text</t>
   </si>
@@ -270,18 +270,6 @@
   </si>
   <si>
     <t>org</t>
-  </si>
-  <si>
-    <t>nl</t>
-  </si>
-  <si>
-    <t>euro</t>
-  </si>
-  <si>
-    <t>earth</t>
-  </si>
-  <si>
-    <t>universe</t>
   </si>
 </sst>
 </file>
@@ -640,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -684,32 +672,6 @@
     <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>82</v>
-      </c>
-      <c r="C4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1682,7 +1644,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>